<commit_message>
Merged PR 5702: M4-79254 Implement option to overrule display's Excel template in Export to Excel popup
Implement option to overrule display's Excel template in Export to Excel popup
</commit_message>
<xml_diff>
--- a/Robot/resources/RobotEaTestExcelTemplate.xlsx
+++ b/Robot/resources/RobotEaTestExcelTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robot\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EveryAngle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFB047BE-53D9-4781-A433-1A7E7D302B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52167416-CCC9-456F-B45C-544B50914D56}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Angle name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>{displayfilters}</t>
+  </si>
+  <si>
+    <t>{displaydescription}</t>
   </si>
   <si>
     <t>Column1</t>
@@ -266,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -337,7 +340,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,20 +939,20 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="78.5546875" customWidth="1"/>
-    <col min="3" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="78.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="78.5703125" customWidth="1"/>
+    <col min="3" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="78.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -966,43 +968,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="17"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="17"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="18"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>2</v>
       </c>
@@ -1014,23 +1016,23 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
@@ -1039,22 +1041,26 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>16</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="19"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -1062,9 +1068,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>9</v>
@@ -1089,16 +1095,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="121.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.88671875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="121.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1111,19 +1117,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>